<commit_message>
custom ARpUIiRC and webappdata
</commit_message>
<xml_diff>
--- a/InputData/elec/ARpUIiRC/Ann Ret per Unit Inc in Relative Cost.xlsx
+++ b/InputData/elec/ARpUIiRC/Ann Ret per Unit Inc in Relative Cost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\Canada\canada-eps\InputData\elec\ARpUIiRC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\Canada\eps-canada\InputData\elec\ARpUIiRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2F380F-D34D-49ED-AE9D-7EF7D8C43BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF397E0E-8333-47D1-958B-E0783D554471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="495" windowWidth="16410" windowHeight="16905" tabRatio="606" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="606" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,12 @@
     <sheet name="Table 3" sheetId="20" r:id="rId6"/>
     <sheet name="Table 9" sheetId="21" r:id="rId7"/>
     <sheet name="Weighting" sheetId="8" r:id="rId8"/>
-    <sheet name="ARpUIiRC" sheetId="2" r:id="rId9"/>
+    <sheet name="us-syc" sheetId="24" r:id="rId9"/>
+    <sheet name="canada-syc" sheetId="23" r:id="rId10"/>
+    <sheet name="ARpUIiRC" sheetId="2" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <definedNames>
     <definedName name="dollars_2020_2012">[1]About!$A$103</definedName>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2546" uniqueCount="1319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2590" uniqueCount="1328">
   <si>
     <t>ARpUIiRC Annual Retirement per Unit Increase in Relative Cost</t>
   </si>
@@ -4025,15 +4027,44 @@
   <si>
     <t>Table 3 for Reference and High Oil and Gas Supply cases (fuel prices) and Table 9 for Refernce and High Oil and Gas Supply case capacity</t>
   </si>
+  <si>
+    <t>Start Year Capacities (MW)</t>
+  </si>
+  <si>
+    <t>preexisting</t>
+  </si>
+  <si>
+    <t>preexisting nonretiring (not used in U.S. dataset)</t>
+  </si>
+  <si>
+    <t>newly built</t>
+  </si>
+  <si>
+    <t>preexisting nonretiring</t>
+  </si>
+  <si>
+    <t>ratio to US values</t>
+  </si>
+  <si>
+    <t>adjusted ARpUiRC values</t>
+  </si>
+  <si>
+    <t>original ARpUiRC values</t>
+  </si>
+  <si>
+    <t>&lt;-manually adjusted</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -4188,7 +4219,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
@@ -4209,8 +4240,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4277,9 +4309,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="11">
     <cellStyle name="Body: normal cell" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma" xfId="10" builtinId="3"/>
     <cellStyle name="Font: Calibri, 9pt regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Footnotes: top row" xfId="8" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
@@ -7659,6 +7696,620 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F5564F-D507-42F5-9570-B4518A756B6A}">
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1320</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1322</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>1324</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>1326</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2">
+        <v>8929</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7">
+        <f>B2/'us-syc'!B2</f>
+        <v>4.0584149955456977E-2</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3500</v>
+      </c>
+      <c r="H2" s="39">
+        <f>IFERROR(G2*F2,0)</f>
+        <v>142.04452484409941</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>15649</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <f>B3/SUM('us-syc'!B3,'us-syc'!C3)</f>
+        <v>4.7162532774780747E-2</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3686</v>
+      </c>
+      <c r="H3" s="39">
+        <f t="shared" ref="H3:H17" si="0">IFERROR(G3*F3,0)</f>
+        <v>173.84109580784184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>13338</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
+        <f>B4/'us-syc'!B4</f>
+        <v>0.1359369744901599</v>
+      </c>
+      <c r="G4" s="3">
+        <v>6000</v>
+      </c>
+      <c r="H4" s="39">
+        <v>500</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>81383</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
+        <f>B5/'us-syc'!B5</f>
+        <v>1.0238916008253234</v>
+      </c>
+      <c r="G5" s="3">
+        <v>581</v>
+      </c>
+      <c r="H5" s="39">
+        <f t="shared" si="0"/>
+        <v>594.88102007951284</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <v>12782</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <f>B6/'us-syc'!B6</f>
+        <v>0.1235883353960396</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7">
+        <v>2719</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7">
+        <f>B7/'us-syc'!B7</f>
+        <v>7.7088826514700462E-2</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7">
+        <f>B8/'us-syc'!B8</f>
+        <v>5.6882821387940839E-4</v>
+      </c>
+      <c r="G8" s="3">
+        <v>5699</v>
+      </c>
+      <c r="H8" s="39">
+        <f t="shared" si="0"/>
+        <v>3.2417519908987482</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9">
+        <v>2460</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7">
+        <f>B9/'us-syc'!B9</f>
+        <v>0.50132463827185658</v>
+      </c>
+      <c r="G9" s="3">
+        <v>5938</v>
+      </c>
+      <c r="H9" s="39">
+        <f t="shared" si="0"/>
+        <v>2976.8657020582846</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7">
+        <f>B10/'us-syc'!B10</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>2435</v>
+      </c>
+      <c r="H10" s="39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11">
+        <v>3615</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
+        <f>B11/'us-syc'!B11</f>
+        <v>0.12857447716602646</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12">
+        <v>6928</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7">
+        <f>B12/'us-syc'!B12</f>
+        <v>5.4380332655672339E-2</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7">
+        <f>B13/'us-syc'!B13</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>3679</v>
+      </c>
+      <c r="H13" s="39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7">
+        <f>B14/'us-syc'!B14</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7" t="e">
+        <f>B15/'us-syc'!B15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7" t="e">
+        <f>B16/'us-syc'!B16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="7">
+        <f>B17/'us-syc'!B17</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
+        <v>5200</v>
+      </c>
+      <c r="H17" s="39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2">
+        <f>'canada-syc'!H2</f>
+        <v>142.04452484409941</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <f>'canada-syc'!H3</f>
+        <v>173.84109580784184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <f>'canada-syc'!H4</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <f>'canada-syc'!H5</f>
+        <v>594.88102007951284</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <f>'canada-syc'!H6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7">
+        <f>'canada-syc'!H7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <f>'canada-syc'!H8</f>
+        <v>3.2417519908987482</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9">
+        <f>'canada-syc'!H9</f>
+        <v>2976.8657020582846</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <f>'canada-syc'!H10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11">
+        <f>'canada-syc'!H11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12">
+        <f>'canada-syc'!H12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13">
+        <f>'canada-syc'!H13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14">
+        <f>'canada-syc'!H14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <f>'canada-syc'!H15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16">
+        <f>'canada-syc'!H16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17">
+        <f>'canada-syc'!H17</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F6BE89-089C-45B7-8D41-7E0BDC91B5BE}">
   <dimension ref="A1:AH2841"/>
@@ -16636,6 +17287,15 @@
     <row r="2841" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B2598:AG2598"/>
+    <mergeCell ref="B2719:AG2719"/>
+    <mergeCell ref="B2837:AG2837"/>
+    <mergeCell ref="B1945:AG1945"/>
+    <mergeCell ref="B2031:AG2031"/>
+    <mergeCell ref="B2153:AG2153"/>
+    <mergeCell ref="B2317:AG2317"/>
+    <mergeCell ref="B2419:AG2419"/>
+    <mergeCell ref="B2509:AG2509"/>
     <mergeCell ref="B1698:AG1698"/>
     <mergeCell ref="B87:AG87"/>
     <mergeCell ref="B112:AG112"/>
@@ -16648,15 +17308,6 @@
     <mergeCell ref="B1390:AG1390"/>
     <mergeCell ref="B1502:AG1502"/>
     <mergeCell ref="B1604:AG1604"/>
-    <mergeCell ref="B2598:AG2598"/>
-    <mergeCell ref="B2719:AG2719"/>
-    <mergeCell ref="B2837:AG2837"/>
-    <mergeCell ref="B1945:AG1945"/>
-    <mergeCell ref="B2031:AG2031"/>
-    <mergeCell ref="B2153:AG2153"/>
-    <mergeCell ref="B2317:AG2317"/>
-    <mergeCell ref="B2419:AG2419"/>
-    <mergeCell ref="B2509:AG2509"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -63860,160 +64511,251 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
-    <tabColor theme="3"/>
-  </sheetPr>
-  <dimension ref="A1:B17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61E9B258-A85B-4CC3-89E8-D3AF6579C073}">
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1319</v>
+      </c>
       <c r="B1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1320</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="3">
-        <f>'Coal and Nuclear Calibration'!B28</f>
-        <v>3500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>220012</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="3">
-        <f>$B$2*Weighting!B104</f>
-        <v>3686.1389187979057</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>68647</v>
+      </c>
+      <c r="C3">
+        <v>263163</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="3">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>98119</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="3">
-        <f>$B$2*Weighting!B106</f>
-        <v>581.05247074433396</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>79484</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>103424</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>35271</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="3">
-        <f>$B$2*Weighting!B109</f>
-        <v>5699.3703019089717</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1758</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="3">
-        <f>$B$2*Weighting!B110</f>
-        <v>5938.2040456125651</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>4907</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="3">
-        <f>$B$2*Weighting!B111</f>
-        <v>2435.1147753973464</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="B10">
+        <v>2506</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="B11">
+        <v>28116</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>127399</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="3">
-        <f>$B$2*Weighting!B114</f>
-        <v>3679.2702913559947</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>6798</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>29</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="3">
-        <f>$B$2*Weighting!B118</f>
-        <v>5200.1373040599537</v>
+      <c r="B17">
+        <v>1760</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>